<commit_message>
FINAL UPDATE for ME701
</commit_message>
<xml_diff>
--- a/Project/reichenberger_michael_code/MPI_Comparison.xlsx
+++ b/Project/reichenberger_michael_code/MPI_Comparison.xlsx
@@ -128,14 +128,14 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -196,11 +196,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="211519568"/>
-        <c:axId val="303936952"/>
+        <c:axId val="280852560"/>
+        <c:axId val="280852952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="211519568"/>
+        <c:axId val="280852560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -229,7 +229,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -242,10 +242,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US">
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:rPr>
+                  <a:rPr lang="en-US"/>
                   <a:t>Number of Nodes</a:t>
                 </a:r>
               </a:p>
@@ -265,7 +262,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -289,10 +286,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -303,7 +297,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -318,12 +312,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303936952"/>
+        <c:crossAx val="280852952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="303936952"/>
+        <c:axId val="280852952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -350,7 +345,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -363,10 +358,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US">
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:rPr>
+                  <a:rPr lang="en-US"/>
                   <a:t>Execution Time</a:t>
                 </a:r>
               </a:p>
@@ -386,7 +378,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -410,10 +402,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -424,7 +413,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -439,9 +428,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211519568"/>
+        <c:crossAx val="280852560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="10"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -475,7 +465,420 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1200">
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nodes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.083333333333327E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>60.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.67</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="20"/>
+        <c:axId val="359220952"/>
+        <c:axId val="359224480"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="359220952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Number of Nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="359224480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="359224480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Execution Time (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="359220952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -528,6 +931,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1044,20 +1487,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1071,6 +2017,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>128587</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>128587</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1368,8 +2344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>